<commit_message>
worked on PIIDs for RSK, MC, PLAN
</commit_message>
<xml_diff>
--- a/PIID/MC.xlsx
+++ b/PIID/MC.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>MC</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Verified- Y/N</t>
   </si>
   <si>
-    <t>GGE200</t>
-  </si>
-  <si>
-    <t>CHAR - GGE200-FI/LI</t>
-  </si>
-  <si>
     <t>Level 1</t>
   </si>
   <si>
@@ -85,21 +79,6 @@
   </si>
   <si>
     <t>Doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s:MPP with actual dates of activities to monitor progress against schedule </t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>PM affirmed  mpp updated after completion of task</t>
-  </si>
-  <si>
-    <t>Aff</t>
   </si>
   <si>
     <t>-</t>
@@ -115,15 +94,6 @@
 </t>
   </si>
   <si>
-    <t>i: Issue with are identified in project should be mentioned in issue log with resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s: Team meeting during the projects showing action has been taken against decision </t>
-  </si>
-  <si>
-    <t>s:Document received against affirmation</t>
-  </si>
-  <si>
     <t>Level 2</t>
   </si>
   <si>
@@ -131,9 +101,6 @@
   </si>
   <si>
     <t>Project Plan according to effort estimation</t>
-  </si>
-  <si>
-    <t>s:</t>
   </si>
   <si>
     <t>https://gil.einframe.com/data-capture/development/capprojecttalentmap.aspx?projectid=96</t>
@@ -148,16 +115,10 @@
     <t>Budget Deatails</t>
   </si>
   <si>
-    <t>s:Milestone review with senior management at  the end of each phase</t>
-  </si>
-  <si>
     <t xml:space="preserve">Track the involvement of identified stakeholders and commitments. </t>
   </si>
   <si>
     <t>Team</t>
-  </si>
-  <si>
-    <t>I: Action items are not consolidated at one place and tracked</t>
   </si>
   <si>
     <t>Time Sheet</t>
@@ -166,22 +127,10 @@
     <t>timesheet los for GGE302</t>
   </si>
   <si>
-    <t>s:Monitor stakeholder involvement through Time sheet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monitor the transition to operations and support. </t>
   </si>
   <si>
-    <t>s:Applicable design output with release items</t>
-  </si>
-  <si>
     <t>http://192.168.100.9:8080/svn/DC_DC_Converter/SP10_GGE302/Testing/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s:rivision history mentioned </t>
-  </si>
-  <si>
-    <t>s: Feedback from production has been mentioned in the pilot report</t>
   </si>
   <si>
     <t xml:space="preserve">Take corrective actions when actual results differ significantly from planned results and manage to closure. </t>
@@ -208,19 +157,10 @@
     <t>continuous monitoring of project through status meetings</t>
   </si>
   <si>
-    <t xml:space="preserve">s: Team meeting during the projects showing project plan has been monitored </t>
-  </si>
-  <si>
-    <t>PM affirmed that plan is monitored using MPP and team meeting</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manage critical dependencies and activities. </t>
   </si>
   <si>
     <t>Status review meetings have details about each activity and roadblocks</t>
-  </si>
-  <si>
-    <t>s: Team meeting during the projects showing that dependencies are reviewed and updated</t>
   </si>
   <si>
     <t>GGE302_RSKMTX</t>
@@ -229,16 +169,10 @@
     <t xml:space="preserve">risk matrix for detail </t>
   </si>
   <si>
-    <t>s: in risk matrix ,risk has been identified and plan for mitigation and contingency is mentioned</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monitor the work environment to identify issues. </t>
   </si>
   <si>
     <t>Status review meetings have details about each activity and roadblocks if any, critical dependency. (C69), eg. SMF battery procurement</t>
-  </si>
-  <si>
-    <t>s: Team meeting during the projects showing activities monitor during the meeting</t>
   </si>
   <si>
     <t xml:space="preserve">Manage and resolve issues with affected stakeholders. </t>
@@ -247,19 +181,7 @@
     <t>project metrics report provide every measurement data related to project an their causal analysis for the issues faced,</t>
   </si>
   <si>
-    <t>s:Metrics report where analysis the measurement with corrective action</t>
-  </si>
-  <si>
-    <t>LM</t>
-  </si>
-  <si>
     <t>any discrepancy/problem/issue is mentioned in MOM (C-100)</t>
-  </si>
-  <si>
-    <t>s: Team meeting during the projects showing action against the decision taken in previous meeting</t>
-  </si>
-  <si>
-    <t>W: The actions to resolve identified issues are not explicit.</t>
   </si>
   <si>
     <t>S</t>
@@ -281,6 +203,12 @@
   </si>
   <si>
     <t>SVN repository for project</t>
+  </si>
+  <si>
+    <t>GGE302</t>
+  </si>
+  <si>
+    <t>CHAR - GGE302-FI/LI</t>
   </si>
 </sst>
 </file>
@@ -1608,11 +1536,11 @@
   </sheetPr>
   <dimension ref="A1:R276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A33"/>
+      <selection pane="bottomRight" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1681,54 +1609,50 @@
         <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" ht="38.25">
+    <row r="4" spans="1:18" ht="15.75">
       <c r="A4" s="56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="58">
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="str">
         <f>IF(LEN(E4)&gt;5,IF(LEN(K4&amp;L4&amp;M4)&gt;=1,"OK","Check"),"-")</f>
         <v>OK</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="14" t="str">
         <f t="shared" ref="I4:I5" si="0">IF(MID(H4,2,1)=":",LEFT(H4,1),"-")</f>
-        <v>s</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J4" s="14"/>
       <c r="K4" s="8" t="str">
         <f>IF(COUNTIFS($E4,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L4" s="8" t="str">
         <f t="shared" ref="L4:M19" si="1">IF(COUNTIFS($E4,"*"&amp;L$3&amp;"*")&gt;=1,"X","")</f>
@@ -1738,15 +1662,13 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="58"/>
       <c r="R4" s="56"/>
     </row>
-    <row r="5" spans="1:18" ht="25.5">
+    <row r="5" spans="1:18" ht="15.75">
       <c r="A5" s="56"/>
       <c r="B5" s="59"/>
       <c r="C5" s="65"/>
@@ -1755,20 +1677,14 @@
         <v>-</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J5" s="14"/>
       <c r="K5" s="8" t="str">
         <f t="shared" ref="K5:M68" si="3">IF(COUNTIFS($E5,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v/>
@@ -1800,7 +1716,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="8" t="str">
@@ -2247,34 +2163,30 @@
         <v>1.2</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>i</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J19" s="14"/>
       <c r="K19" s="8" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L19" s="8" t="str">
         <f t="shared" si="1"/>
@@ -2284,15 +2196,13 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="N19" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="58"/>
       <c r="R19" s="56"/>
     </row>
-    <row r="20" spans="1:18" ht="38.25">
+    <row r="20" spans="1:18" ht="15.75">
       <c r="A20" s="56"/>
       <c r="B20" s="59"/>
       <c r="C20" s="66"/>
@@ -2302,19 +2212,13 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J20" s="14"/>
       <c r="K20" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2343,19 +2247,13 @@
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J21" s="14"/>
       <c r="K21" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2492,7 +2390,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="8" t="str">
@@ -2795,40 +2693,36 @@
     </row>
     <row r="34" spans="1:18" ht="38.25" customHeight="1">
       <c r="A34" s="56" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B34" s="58">
         <v>2.1</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D34" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H34" s="5"/>
       <c r="I34" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J34" s="14"/>
       <c r="K34" s="8" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L34" s="8" t="str">
         <f t="shared" si="3"/>
@@ -2838,9 +2732,7 @@
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="N34" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N34" s="11"/>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="58"/>
@@ -2855,24 +2747,20 @@
         <v>OK</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H35" s="5"/>
       <c r="I35" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J35" s="14"/>
       <c r="K35" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2891,7 +2779,7 @@
       <c r="Q35" s="59"/>
       <c r="R35" s="56"/>
     </row>
-    <row r="36" spans="1:18" ht="38.25">
+    <row r="36" spans="1:18" ht="15.75">
       <c r="A36" s="56"/>
       <c r="B36" s="59"/>
       <c r="C36" s="65"/>
@@ -2900,24 +2788,20 @@
         <v>OK</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J36" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J36" s="14"/>
       <c r="K36" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2946,17 +2830,13 @@
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G37" s="11"/>
       <c r="H37" s="5"/>
       <c r="I37" s="14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J37" s="14"/>
       <c r="K37" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2985,17 +2865,13 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G38" s="11"/>
       <c r="H38" s="5"/>
       <c r="I38" s="14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="J38" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J38" s="14"/>
       <c r="K38" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3370,31 +3246,27 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C49" s="65" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D49" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H49" s="5"/>
       <c r="I49" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>I</v>
-      </c>
-      <c r="J49" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J49" s="14"/>
       <c r="K49" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3407,15 +3279,13 @@
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="N49" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N49" s="11"/>
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="58"/>
       <c r="R49" s="56"/>
     </row>
-    <row r="50" spans="1:18" ht="38.25">
+    <row r="50" spans="1:18" ht="15.75">
       <c r="A50" s="56"/>
       <c r="B50" s="59"/>
       <c r="C50" s="65"/>
@@ -3424,24 +3294,20 @@
         <v>OK</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>44</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H50" s="5"/>
       <c r="I50" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J50" s="14"/>
       <c r="K50" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3470,17 +3336,13 @@
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G51" s="11"/>
       <c r="H51" s="8"/>
       <c r="I51" s="14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="J51" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J51" s="14"/>
       <c r="K51" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3925,7 +3787,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C64" s="67" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D64" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3958,7 +3820,7 @@
       <c r="Q64" s="58"/>
       <c r="R64" s="56"/>
     </row>
-    <row r="65" spans="1:18" ht="25.5">
+    <row r="65" spans="1:18" ht="15.75">
       <c r="A65" s="56"/>
       <c r="B65" s="59"/>
       <c r="C65" s="67"/>
@@ -3967,27 +3829,23 @@
         <v>OK</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H65" s="5"/>
       <c r="I65" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J65" s="14"/>
       <c r="K65" s="8" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L65" s="8" t="str">
         <f t="shared" si="3"/>
@@ -3997,9 +3855,7 @@
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="N65" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N65" s="11"/>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
       <c r="Q65" s="59"/>
@@ -4014,27 +3870,23 @@
         <v>OK</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H66" s="5"/>
       <c r="I66" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J66" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J66" s="14"/>
       <c r="K66" s="8" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L66" s="8" t="str">
         <f t="shared" si="3"/>
@@ -4061,18 +3913,14 @@
       <c r="E67" s="9"/>
       <c r="F67" s="7"/>
       <c r="G67" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H67" s="8"/>
       <c r="I67" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
-      </c>
-      <c r="J67" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J67" s="14"/>
       <c r="K67" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4101,17 +3949,13 @@
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="7"/>
-      <c r="G68" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G68" s="11"/>
       <c r="H68" s="5"/>
       <c r="I68" s="14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="J68" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J68" s="14"/>
       <c r="K68" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4486,34 +4330,30 @@
         <v>2.4</v>
       </c>
       <c r="C79" s="66" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D79" s="5" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>33</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H79" s="8"/>
       <c r="I79" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J79" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J79" s="14"/>
       <c r="K79" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L79" s="8" t="str">
         <f t="shared" si="7"/>
@@ -4523,9 +4363,7 @@
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="N79" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N79" s="11"/>
       <c r="O79" s="11"/>
       <c r="P79" s="11"/>
       <c r="Q79" s="58"/>
@@ -4540,25 +4378,23 @@
         <v>OK</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H80" s="8"/>
       <c r="I80" s="14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="J80" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J80" s="14"/>
       <c r="K80" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L80" s="8" t="str">
         <f t="shared" si="7"/>
@@ -4584,17 +4420,13 @@
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G81" s="11"/>
       <c r="H81" s="8"/>
       <c r="I81" s="14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="J81" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J81" s="14"/>
       <c r="K81" s="8" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5035,40 +4867,36 @@
     </row>
     <row r="94" spans="1:18" ht="12.75" customHeight="1">
       <c r="A94" s="57" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B94" s="61">
         <v>3.1</v>
       </c>
       <c r="C94" s="66" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D94" s="5" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H94" s="5"/>
       <c r="I94" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J94" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J94" s="14"/>
       <c r="K94" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L94" s="8" t="str">
         <f t="shared" si="7"/>
@@ -5078,15 +4906,13 @@
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="N94" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N94" s="11"/>
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
       <c r="Q94" s="61"/>
       <c r="R94" s="57"/>
     </row>
-    <row r="95" spans="1:18" ht="38.25">
+    <row r="95" spans="1:18" ht="25.5">
       <c r="A95" s="57"/>
       <c r="B95" s="62"/>
       <c r="C95" s="66"/>
@@ -5095,27 +4921,23 @@
         <v>OK</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H95" s="5"/>
       <c r="I95" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J95" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J95" s="14"/>
       <c r="K95" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L95" s="8" t="str">
         <f t="shared" si="7"/>
@@ -5140,20 +4962,14 @@
         <v>-</v>
       </c>
       <c r="E96" s="9"/>
-      <c r="F96" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G96" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="F96" s="16"/>
+      <c r="G96" s="11"/>
       <c r="H96" s="8"/>
       <c r="I96" s="14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="J96" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J96" s="14"/>
       <c r="K96" s="8" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5592,40 +5408,36 @@
       <c r="Q108" s="63"/>
       <c r="R108" s="57"/>
     </row>
-    <row r="109" spans="1:18" ht="51">
+    <row r="109" spans="1:18" ht="38.25">
       <c r="A109" s="57"/>
       <c r="B109" s="61">
         <v>3.2</v>
       </c>
       <c r="C109" s="66" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D109" s="5" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H109" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H109" s="5"/>
       <c r="I109" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J109" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J109" s="14"/>
       <c r="K109" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L109" s="8" t="str">
         <f t="shared" si="7"/>
@@ -5635,15 +5447,13 @@
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="N109" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N109" s="11"/>
       <c r="O109" s="11"/>
       <c r="P109" s="11"/>
       <c r="Q109" s="61"/>
       <c r="R109" s="57"/>
     </row>
-    <row r="110" spans="1:18" ht="51">
+    <row r="110" spans="1:18" ht="15.75">
       <c r="A110" s="57"/>
       <c r="B110" s="62"/>
       <c r="C110" s="66"/>
@@ -5652,27 +5462,23 @@
         <v>OK</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H110" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H110" s="5"/>
       <c r="I110" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J110" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J110" s="14"/>
       <c r="K110" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L110" s="8" t="str">
         <f t="shared" si="7"/>
@@ -5698,17 +5504,13 @@
       </c>
       <c r="E111" s="9"/>
       <c r="F111" s="7"/>
-      <c r="G111" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G111" s="11"/>
       <c r="H111" s="8"/>
       <c r="I111" s="14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="J111" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J111" s="14"/>
       <c r="K111" s="8" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6153,34 +5955,30 @@
         <v>3.3</v>
       </c>
       <c r="C124" s="66" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D124" s="5" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H124" s="5" t="s">
-        <v>68</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H124" s="5"/>
       <c r="I124" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>s</v>
-      </c>
-      <c r="J124" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J124" s="14"/>
       <c r="K124" s="8" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L124" s="8" t="str">
         <f t="shared" si="7"/>
@@ -6190,9 +5988,7 @@
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="N124" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="N124" s="11"/>
       <c r="O124" s="11"/>
       <c r="P124" s="11"/>
       <c r="Q124" s="61"/>
@@ -6208,17 +6004,13 @@
       </c>
       <c r="E125" s="9"/>
       <c r="F125" s="7"/>
-      <c r="G125" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G125" s="11"/>
       <c r="H125" s="8"/>
       <c r="I125" s="14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="J125" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="J125" s="14"/>
       <c r="K125" s="8" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6698,34 +6490,30 @@
         <v>3.4</v>
       </c>
       <c r="C139" s="66" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D139" s="5" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H139" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H139" s="8"/>
       <c r="I139" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>s</v>
-      </c>
-      <c r="J139" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J139" s="14"/>
       <c r="K139" s="8" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L139" s="8" t="str">
         <f t="shared" si="10"/>
@@ -6735,15 +6523,13 @@
         <f t="shared" si="10"/>
         <v>X</v>
       </c>
-      <c r="N139" s="11" t="s">
-        <v>72</v>
-      </c>
+      <c r="N139" s="11"/>
       <c r="O139" s="11"/>
       <c r="P139" s="11"/>
       <c r="Q139" s="61"/>
       <c r="R139" s="57"/>
     </row>
-    <row r="140" spans="1:18" ht="51">
+    <row r="140" spans="1:18" ht="25.5">
       <c r="A140" s="57"/>
       <c r="B140" s="62"/>
       <c r="C140" s="66"/>
@@ -6752,27 +6538,23 @@
         <v>OK</v>
       </c>
       <c r="E140" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H140" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H140" s="5"/>
       <c r="I140" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>s</v>
-      </c>
-      <c r="J140" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J140" s="14"/>
       <c r="K140" s="8" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L140" s="8" t="str">
         <f t="shared" si="10"/>
@@ -6788,7 +6570,7 @@
       <c r="Q140" s="62"/>
       <c r="R140" s="57"/>
     </row>
-    <row r="141" spans="1:18" ht="38.25">
+    <row r="141" spans="1:18" ht="15.75">
       <c r="A141" s="57"/>
       <c r="B141" s="62"/>
       <c r="C141" s="66"/>
@@ -6798,19 +6580,13 @@
       </c>
       <c r="E141" s="9"/>
       <c r="F141" s="7"/>
-      <c r="G141" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H141" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="G141" s="11"/>
+      <c r="H141" s="5"/>
       <c r="I141" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>W</v>
-      </c>
-      <c r="J141" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J141" s="14"/>
       <c r="K141" s="8" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -8627,7 +8403,7 @@
       <c r="G193" s="11"/>
       <c r="H193" s="8"/>
       <c r="I193" s="14" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="J193" s="14"/>
       <c r="K193" s="8" t="str">
@@ -11463,7 +11239,7 @@
     </row>
     <row r="275" spans="1:18" ht="15.75" customHeight="1">
       <c r="A275" s="51" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B275" s="51"/>
       <c r="C275" s="51"/>

</xml_diff>